<commit_message>
:construction: Add a naive synergy score
</commit_message>
<xml_diff>
--- a/raw_asset/card_statistic/card_synergy.xlsx
+++ b/raw_asset/card_statistic/card_synergy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\桌面\git_repo\agricola.tools\raw_asset\card_statistic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61368093-6E4F-40BF-943A-70AD9110321F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243D9BBA-B9E1-448A-898F-97E75D820724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="612">
   <si>
     <t>Inner Districts Director</t>
   </si>
@@ -1633,10 +1633,6 @@
   </si>
   <si>
     <t>field</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>day laborer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1941,6 +1937,66 @@
   </si>
   <si>
     <t>wood clay VP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>more</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fishing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zz_TEST14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day_laborer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2017,7 +2073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2037,6 +2093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -2107,10 +2164,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3111D54A-CD6F-4C22-82FE-7C97485521AC}" name="表格3" displayName="表格3" ref="A1:J504" totalsRowShown="0">
-  <autoFilter ref="A1:J504" xr:uid="{7622DB37-7C1D-4226-A965-FF833A148354}"/>
-  <sortState ref="A2:H504">
-    <sortCondition ref="A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3111D54A-CD6F-4C22-82FE-7C97485521AC}" name="表格3" displayName="表格3" ref="A1:J513" totalsRowShown="0">
+  <autoFilter ref="A1:J513" xr:uid="{7622DB37-7C1D-4226-A965-FF833A148354}"/>
+  <sortState ref="A2:J513">
+    <sortCondition ref="A1:A513"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3449FEBB-0302-457A-82D3-2237CEA273CE}" name="Card Name" dataDxfId="9"/>
@@ -2407,7 +2464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAA3AAE-FB38-4AC7-BBDB-9FEAF49BAD3D}">
-  <dimension ref="A1:J504"/>
+  <dimension ref="A1:J513"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -2457,7 +2514,7 @@
         <v>516</v>
       </c>
       <c r="J1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2523,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -2632,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G6">
         <f>0</f>
@@ -2676,10 +2733,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J7" s="1">
         <f>0</f>
@@ -2703,7 +2760,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G8">
         <f>0</f>
@@ -2895,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -3006,7 +3063,7 @@
         <v>522</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>523</v>
+        <v>611</v>
       </c>
       <c r="J16" s="1">
         <f>0</f>
@@ -3072,14 +3129,14 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G18">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -3108,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G19">
         <f>0</f>
@@ -3192,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3486,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -3516,20 +3573,20 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G30">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -3550,14 +3607,14 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G31">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -3625,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G33">
         <f>0</f>
@@ -3695,14 +3752,14 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G35">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -3777,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
@@ -3992,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -4028,7 +4085,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -4057,14 +4114,14 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G45">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I45" s="1">
         <v>0</v>
@@ -4254,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -4282,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
@@ -4358,13 +4415,13 @@
         <v>0</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I53" s="9">
         <v>0</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -4399,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -4462,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -4578,10 +4635,10 @@
         <v>0</v>
       </c>
       <c r="H59" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="J59" s="1">
         <f>0</f>
@@ -4615,13 +4672,13 @@
         <v>0</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -4649,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -4686,13 +4743,13 @@
         <v>1</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I62" s="1">
         <v>0</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -4721,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -4756,7 +4813,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -4792,7 +4849,7 @@
         <v>0</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I65" s="1">
         <v>0</v>
@@ -4944,10 +5001,10 @@
         <v>0</v>
       </c>
       <c r="H69" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>551</v>
       </c>
       <c r="J69" s="1">
         <f>0</f>
@@ -4981,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
@@ -5018,7 +5075,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
@@ -5055,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I72" s="1">
         <v>0</v>
@@ -5092,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I73" s="1">
         <v>0</v>
@@ -5128,7 +5185,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I74" s="1">
         <v>0</v>
@@ -5164,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I75" s="1">
         <v>0</v>
@@ -5200,7 +5257,7 @@
         <v>0</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
@@ -5237,10 +5294,10 @@
         <v>0</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J77" s="1">
         <f>0</f>
@@ -5274,7 +5331,7 @@
         <v>0</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I78" s="1">
         <v>0</v>
@@ -5310,7 +5367,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I79" s="1">
         <v>0</v>
@@ -5346,10 +5403,10 @@
         <v>0</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J80" s="1">
         <f>0</f>
@@ -5381,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I81" s="1">
         <v>0</v>
@@ -5417,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I82" s="1">
         <v>0</v>
@@ -5453,7 +5510,7 @@
         <v>0</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I83" s="1">
         <v>0</v>
@@ -5528,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I85" s="1">
         <v>0</v>
@@ -5564,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I86" s="1">
         <v>0</v>
@@ -5640,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I88" s="1">
         <v>0</v>
@@ -5669,14 +5726,14 @@
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G89">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I89" s="1">
         <v>0</v>
@@ -5751,10 +5808,10 @@
         <v>0</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J91" s="1">
         <f>0</f>
@@ -5787,14 +5844,14 @@
         <v>0</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I92" s="1">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -5862,7 +5919,7 @@
         <v>0</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I94" s="1">
         <v>0</v>
@@ -5897,13 +5954,13 @@
         <v>0</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I95" s="1">
         <v>0</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -5932,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I96" s="1">
         <v>0</v>
@@ -5968,7 +6025,7 @@
         <v>0</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I97" s="1">
         <v>0</v>
@@ -6003,7 +6060,7 @@
         <v>0</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I98" s="1">
         <v>0</v>
@@ -6039,7 +6096,7 @@
         <v>0</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I99" s="1">
         <v>0</v>
@@ -6074,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I100" s="1">
         <v>0</v>
@@ -6109,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I101" s="1">
         <v>0</v>
@@ -6145,10 +6202,10 @@
         <v>0</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J102" s="1">
         <f>0</f>
@@ -6181,7 +6238,7 @@
         <v>0</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I103" s="1">
         <v>0</v>
@@ -6217,10 +6274,10 @@
         <v>0</v>
       </c>
       <c r="H104" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="I104" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>570</v>
       </c>
       <c r="J104" s="1">
         <f>0</f>
@@ -6253,7 +6310,7 @@
         <v>0</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I105" s="1">
         <v>0</v>
@@ -6288,7 +6345,7 @@
         <v>0</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I106" s="1">
         <v>0</v>
@@ -6323,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I107" s="1">
         <v>0</v>
@@ -6360,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I108" s="1">
         <v>0</v>
@@ -6396,10 +6453,10 @@
         <v>0</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J109" s="1">
         <f>0</f>
@@ -6432,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="H110" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I110" s="1">
         <v>0</v>
@@ -6467,7 +6524,7 @@
         <v>0</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I111" s="1">
         <v>0</v>
@@ -6496,14 +6553,14 @@
         <v>0</v>
       </c>
       <c r="F112" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G112">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I112" s="1">
         <v>0</v>
@@ -6538,10 +6595,10 @@
         <v>0</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J113" s="1">
         <f>0</f>
@@ -6573,13 +6630,13 @@
         <v>0</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>523</v>
+        <v>611</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
@@ -6602,14 +6659,14 @@
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G115">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I115" s="1">
         <v>0</v>
@@ -6645,7 +6702,7 @@
         <v>0</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I116" s="1">
         <v>0</v>
@@ -6680,7 +6737,7 @@
         <v>0</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I117" s="1">
         <v>0</v>
@@ -6756,7 +6813,7 @@
         <v>0</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I119" s="1">
         <v>0</v>
@@ -6785,14 +6842,14 @@
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G120">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I120" s="1">
         <v>0</v>
@@ -6827,7 +6884,7 @@
         <v>0</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I121" s="1">
         <v>0</v>
@@ -6896,17 +6953,17 @@
         <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G123">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H123" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J123" s="1">
         <f>0</f>
@@ -6939,7 +6996,7 @@
         <v>0</v>
       </c>
       <c r="H124" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I124" s="1">
         <v>0</v>
@@ -6967,14 +7024,14 @@
         <v>0</v>
       </c>
       <c r="F125" t="s">
+        <v>575</v>
+      </c>
+      <c r="G125">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H125" s="6" t="s">
         <v>576</v>
-      </c>
-      <c r="G125">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H125" s="6" t="s">
-        <v>577</v>
       </c>
       <c r="I125" s="1">
         <v>0</v>
@@ -7010,10 +7067,10 @@
         <v>0</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J126" s="1">
         <f>0</f>
@@ -7046,7 +7103,7 @@
         <v>0</v>
       </c>
       <c r="H127" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I127" s="1">
         <v>0</v>
@@ -7075,14 +7132,14 @@
         <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G128">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I128" s="1">
         <v>0</v>
@@ -7112,14 +7169,14 @@
         <v>0</v>
       </c>
       <c r="F129" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G129">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I129" s="1">
         <v>0</v>
@@ -7155,7 +7212,7 @@
         <v>0</v>
       </c>
       <c r="H130" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I130" s="1">
         <v>0</v>
@@ -7192,7 +7249,7 @@
         <v>1</v>
       </c>
       <c r="H131" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I131" s="1">
         <v>0</v>
@@ -7267,7 +7324,7 @@
         <v>0</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I133" s="1">
         <v>0</v>
@@ -7304,7 +7361,7 @@
         <v>0</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I134" s="1">
         <v>0</v>
@@ -7341,7 +7398,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I135" s="1">
         <v>0</v>
@@ -7416,10 +7473,10 @@
         <v>0</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J137" s="1">
         <f>0</f>
@@ -7453,7 +7510,7 @@
         <v>1</v>
       </c>
       <c r="H138" s="10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I138" s="1">
         <v>0</v>
@@ -7489,7 +7546,7 @@
         <v>0</v>
       </c>
       <c r="H139" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I139" s="1">
         <v>0</v>
@@ -7518,14 +7575,14 @@
         <v>0</v>
       </c>
       <c r="F140" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G140">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H140" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I140" s="1">
         <v>0</v>
@@ -7561,10 +7618,10 @@
         <v>0</v>
       </c>
       <c r="H141" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>523</v>
+        <v>611</v>
       </c>
       <c r="J141" s="1">
         <f>0</f>
@@ -7598,7 +7655,7 @@
         <v>0</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I142" s="1">
         <v>0</v>
@@ -7627,14 +7684,14 @@
         <v>0</v>
       </c>
       <c r="F143" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G143">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H143" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I143" s="1">
         <v>0</v>
@@ -7670,13 +7727,13 @@
         <v>0</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I144" s="1">
         <v>0</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.3">
@@ -7698,14 +7755,14 @@
         <v>0</v>
       </c>
       <c r="F145" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G145">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H145" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I145" s="1">
         <v>0</v>
@@ -7741,7 +7798,7 @@
         <v>0</v>
       </c>
       <c r="H146" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I146" s="1">
         <v>0</v>
@@ -7776,7 +7833,7 @@
         <v>0</v>
       </c>
       <c r="H147" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I147" s="1">
         <v>0</v>
@@ -7811,7 +7868,7 @@
         <v>0</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I148" s="1">
         <v>0</v>
@@ -7846,7 +7903,7 @@
         <v>0</v>
       </c>
       <c r="H149" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I149" s="1">
         <v>0</v>
@@ -7875,14 +7932,14 @@
         <v>0</v>
       </c>
       <c r="F150" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G150">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H150" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I150" s="1">
         <v>0</v>
@@ -7919,7 +7976,7 @@
         <v>0</v>
       </c>
       <c r="H151" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I151" s="1">
         <v>0</v>
@@ -7994,7 +8051,7 @@
         <v>0</v>
       </c>
       <c r="H153" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I153" s="1">
         <v>0</v>
@@ -8030,7 +8087,7 @@
         <v>0</v>
       </c>
       <c r="H154" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I154" s="1">
         <v>0</v>
@@ -8066,7 +8123,7 @@
         <v>0</v>
       </c>
       <c r="H155" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I155" s="1">
         <v>0</v>
@@ -8101,10 +8158,10 @@
         <v>0</v>
       </c>
       <c r="H156" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J156" s="1">
         <f>0</f>
@@ -8137,7 +8194,7 @@
         <v>0</v>
       </c>
       <c r="H157" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I157" s="1">
         <v>0</v>
@@ -8172,7 +8229,7 @@
         <v>0</v>
       </c>
       <c r="H158" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I158" s="1">
         <v>0</v>
@@ -8208,7 +8265,7 @@
         <v>0</v>
       </c>
       <c r="H159" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I159" s="1">
         <v>0</v>
@@ -8244,10 +8301,10 @@
         <v>0</v>
       </c>
       <c r="H160" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J160" s="1">
         <f>0</f>
@@ -8280,10 +8337,10 @@
         <v>0</v>
       </c>
       <c r="H161" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J161" s="1">
         <f>0</f>
@@ -8315,7 +8372,7 @@
         <v>0</v>
       </c>
       <c r="H162" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I162" s="1">
         <v>0</v>
@@ -8345,14 +8402,14 @@
         <v>0</v>
       </c>
       <c r="F163" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G163">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H163" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I163" s="1">
         <v>0</v>
@@ -8388,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="H164" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I164" s="1">
         <f>0</f>
@@ -8425,7 +8482,7 @@
         <v>0</v>
       </c>
       <c r="H165" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I165" s="1">
         <v>0</v>
@@ -8501,7 +8558,7 @@
         <v>0</v>
       </c>
       <c r="H167" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I167" s="1">
         <v>0</v>
@@ -8537,13 +8594,13 @@
         <v>0</v>
       </c>
       <c r="H168" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I168" s="1">
         <v>0</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.3">
@@ -8652,10 +8709,10 @@
         <v>0</v>
       </c>
       <c r="H171" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J171" s="1">
         <f>0</f>
@@ -8664,7 +8721,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B172">
         <f>0</f>
@@ -8727,10 +8784,10 @@
         <v>0</v>
       </c>
       <c r="H173" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J173" s="1">
         <f>0</f>
@@ -8764,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="H174" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I174" s="1">
         <v>0</v>
@@ -8840,7 +8897,7 @@
         <v>0</v>
       </c>
       <c r="H176" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I176" s="1">
         <v>0</v>
@@ -8875,10 +8932,10 @@
         <v>0</v>
       </c>
       <c r="H177" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J177" s="1">
         <f>0</f>
@@ -8904,14 +8961,14 @@
         <v>0</v>
       </c>
       <c r="F178" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G178">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="H178" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I178" s="1">
         <v>0</v>
@@ -8946,7 +9003,7 @@
         <v>0</v>
       </c>
       <c r="H179" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I179" s="1">
         <v>0</v>
@@ -8982,7 +9039,7 @@
         <v>0</v>
       </c>
       <c r="H180" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I180" s="1">
         <v>0</v>
@@ -9018,7 +9075,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I181" s="1">
         <v>0</v>
@@ -9052,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="H182" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I182" s="1">
         <v>0</v>
@@ -9129,13 +9186,13 @@
         <v>0</v>
       </c>
       <c r="H184" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I184" s="1">
         <v>0</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.3">
@@ -9164,7 +9221,7 @@
         <v>0</v>
       </c>
       <c r="H185" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I185" s="1">
         <v>0</v>
@@ -9200,7 +9257,7 @@
         <v>0</v>
       </c>
       <c r="H186" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I186" s="1">
         <v>0</v>
@@ -21930,10 +21987,342 @@
         <v>0</v>
       </c>
     </row>
+    <row r="505" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A505" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B505" s="1">
+        <v>1</v>
+      </c>
+      <c r="C505" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D505" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E505" s="11">
+        <v>1</v>
+      </c>
+      <c r="F505" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G505" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H505" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="I505" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="J505" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="506" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A506" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="B506" s="1">
+        <v>1</v>
+      </c>
+      <c r="C506" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D506" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E506" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="G506" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H506" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I506" s="1">
+        <v>0</v>
+      </c>
+      <c r="J506" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A507" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B507" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C507" s="1">
+        <v>1</v>
+      </c>
+      <c r="D507" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E507" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="G507" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H507" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I507" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="J507" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A508" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B508" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C508" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D508" s="1">
+        <v>1</v>
+      </c>
+      <c r="E508" s="11">
+        <v>1</v>
+      </c>
+      <c r="F508" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G508" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H508" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I508" s="1">
+        <v>0</v>
+      </c>
+      <c r="J508" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="509" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A509" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="B509" s="1">
+        <v>1</v>
+      </c>
+      <c r="C509" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D509" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E509" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="G509" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H509" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="I509" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="J509" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="510" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A510" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="B510" s="1">
+        <v>1</v>
+      </c>
+      <c r="C510" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D510" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E510" s="11">
+        <v>1</v>
+      </c>
+      <c r="F510" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G510" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H510" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="I510" s="1">
+        <v>0</v>
+      </c>
+      <c r="J510" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="511" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A511" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="B511" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C511" s="1">
+        <v>1</v>
+      </c>
+      <c r="D511" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E511" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="G511" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H511" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I511" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J511" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A512" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="B512" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C512" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D512" s="1">
+        <v>1</v>
+      </c>
+      <c r="E512" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F512" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G512" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H512" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I512" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="J512" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A513" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="B513" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C513" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D513" s="1">
+        <v>1</v>
+      </c>
+      <c r="E513" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F513" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G513" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H513" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="I513" s="1">
+        <v>0</v>
+      </c>
+      <c r="J513" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>